<commit_message>
Redefined port/pin layout to allow for future expansion.
</commit_message>
<xml_diff>
--- a/Schematics/Resistor Calculator.xlsx
+++ b/Schematics/Resistor Calculator.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2 Switch" sheetId="1" r:id="rId1"/>
+    <sheet name="3 Switch" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>R1</t>
   </si>
@@ -46,6 +47,24 @@
   </si>
   <si>
     <t>SW1 A2D</t>
+  </si>
+  <si>
+    <t>S1 VDC</t>
+  </si>
+  <si>
+    <t>S1 A2D</t>
+  </si>
+  <si>
+    <t>S2 VDC</t>
+  </si>
+  <si>
+    <t>S2 A2D</t>
+  </si>
+  <si>
+    <t>S3 VDC</t>
+  </si>
+  <si>
+    <t>S3 A2D</t>
   </si>
 </sst>
 </file>
@@ -392,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,4 +493,87 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2200</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2">
+        <v>620</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <f>(B2/(A2+B2))*5</f>
+        <v>1.5625</v>
+      </c>
+      <c r="G2">
+        <f>(B2/(A2+B2))*1024</f>
+        <v>320</v>
+      </c>
+      <c r="H2" s="2">
+        <f>(C2/(A2+B2+C2))*5</f>
+        <v>0.81151832460732987</v>
+      </c>
+      <c r="I2" s="1">
+        <f>(C2/(A2+B2+C2))*1024</f>
+        <v>166.19895287958116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>